<commit_message>
(documentacao) Backlog atualizado com as cores certas
</commit_message>
<xml_diff>
--- a/documentacao/sistema/ProductBacklog.xlsx
+++ b/documentacao/sistema/ProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\Compass.io\documentacao\sistema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6CEC57-B7C9-42D8-964F-749F3F6022D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64153EB4-42F7-4ECE-9659-A5DEFFBB4A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -276,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,27 +299,19 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="0"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,13 +332,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FFFCFCFC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,36 +374,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -425,15 +392,19 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -445,16 +416,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFCFCFC"/>
+      <color rgb="FFFFB219"/>
+      <color rgb="FF1975FF"/>
+      <color rgb="FFF4F4F4"/>
       <color rgb="FFC16407"/>
       <color rgb="FFFFC819"/>
       <color rgb="FFE67708"/>
       <color rgb="FF00297A"/>
       <color rgb="FFE6AF00"/>
       <color rgb="FF8E0000"/>
-      <color rgb="FFF08820"/>
-      <color rgb="FFA20000"/>
-      <color rgb="FF002D86"/>
-      <color rgb="FFF4750C"/>
     </mruColors>
   </colors>
   <extLst>
@@ -731,51 +702,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="112.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="110.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="19" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="7"/>
+    <col min="7" max="9" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -787,14 +757,13 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -806,14 +775,13 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -825,14 +793,13 @@
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -844,14 +811,13 @@
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -863,14 +829,13 @@
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -882,14 +847,13 @@
       <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -901,14 +865,13 @@
       <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -920,14 +883,13 @@
       <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -939,14 +901,13 @@
       <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -958,14 +919,13 @@
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -977,14 +937,13 @@
       <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -996,14 +955,13 @@
       <c r="F13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1015,14 +973,13 @@
       <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+    </row>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1034,14 +991,13 @@
       <c r="F15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1053,14 +1009,13 @@
       <c r="F16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1072,13 +1027,12 @@
       <c r="F17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1090,14 +1044,13 @@
       <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1109,14 +1062,13 @@
       <c r="F19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1128,14 +1080,13 @@
       <c r="F20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1147,14 +1098,13 @@
       <c r="F21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1166,14 +1116,13 @@
       <c r="F22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1185,14 +1134,13 @@
       <c r="F23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1204,13 +1152,12 @@
       <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>3</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1222,14 +1169,13 @@
       <c r="F25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -1241,14 +1187,13 @@
       <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1260,13 +1205,12 @@
       <c r="F27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>4</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1278,14 +1222,13 @@
       <c r="F28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1297,14 +1240,13 @@
       <c r="F29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -1316,14 +1258,13 @@
       <c r="F30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1335,14 +1276,13 @@
       <c r="F31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1354,14 +1294,13 @@
       <c r="F32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1373,14 +1312,13 @@
       <c r="F33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -1392,158 +1330,122 @@
       <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="G47" s="6"/>
-    </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="G49" s="6"/>
-    </row>
-    <row r="50" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="6"/>
-    </row>
-    <row r="51" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G53" s="6"/>
-    </row>
-    <row r="54" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G55" s="6"/>
-    </row>
-    <row r="56" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G56" s="6"/>
-    </row>
-    <row r="57" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G57" s="6"/>
-    </row>
-    <row r="58" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G58" s="6"/>
-    </row>
-    <row r="59" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G59" s="6"/>
-    </row>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">

</xml_diff>